<commit_message>
Minor map changes and updated documentation
</commit_message>
<xml_diff>
--- a/INT0007.UU.PersonEvents/Src/Files/INT0007.UU.PersonEvents.maps.xlsx
+++ b/INT0007.UU.PersonEvents/Src/Files/INT0007.UU.PersonEvents.maps.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ForvantatDeltagandeSkapadEvent" sheetId="4" r:id="rId1"/>
-    <sheet name="RegistreringEvent" sheetId="8" r:id="rId2"/>
+    <sheet name="RegistreringEvent - create" sheetId="8" r:id="rId2"/>
+    <sheet name="LokalStudentEvent" sheetId="9" r:id="rId3"/>
+    <sheet name="RegistreringEvent - validperiod" sheetId="10" r:id="rId4"/>
+    <sheet name="OmegistreringEvent - validpeiod" sheetId="11" r:id="rId5"/>
+    <sheet name="StudentAvlidenMarkering" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
   <si>
     <t>Från</t>
   </si>
@@ -119,13 +123,73 @@
   </si>
   <si>
     <t>[Fornamn], [Efternamn]</t>
+  </si>
+  <si>
+    <t>/LokalStudentEvent</t>
+  </si>
+  <si>
+    <t>Mappning: LokalStudentEvent_To_PersonStudentAccountUpdatedEvent</t>
+  </si>
+  <si>
+    <t>Source: http://schemas.ladok.se/studentinformation</t>
+  </si>
+  <si>
+    <t>Fast värde</t>
+  </si>
+  <si>
+    <t>"PersonStudentAccountUpdatedEvent"</t>
+  </si>
+  <si>
+    <t>StudentUID</t>
+  </si>
+  <si>
+    <t>@newid</t>
+  </si>
+  <si>
+    <t>ErsattAvStudentUID</t>
+  </si>
+  <si>
+    <t>Mappning: RegistreringEnvelope_To_PersonStudentValidPeriodEvent</t>
+  </si>
+  <si>
+    <t>"PersonStudentValidPeriodEvent"</t>
+  </si>
+  <si>
+    <t>används senare att uppdatera giltighetstiden för ett studentkonto</t>
+  </si>
+  <si>
+    <t>Betyder att existerande UID inte ska hanteras vidare! Är upp till mottagande system att hantera konto sammanslagning och dylikt.</t>
+  </si>
+  <si>
+    <t>/OmregistreringEnvelope</t>
+  </si>
+  <si>
+    <t>/OmregistreringEvent</t>
+  </si>
+  <si>
+    <t>Mappning: StudentAvlidenmarkeringEvent_To_PersonEvent</t>
+  </si>
+  <si>
+    <t>/StudentAvlidenmarkeringEvent</t>
+  </si>
+  <si>
+    <t>Fast värde om @avliden = true</t>
+  </si>
+  <si>
+    <t>"PersonStudentDeceasedEvent"</t>
+  </si>
+  <si>
+    <t>"PersonStudentDeceasedRetractionEvent"</t>
+  </si>
+  <si>
+    <t>Fast värde om @avliden = false, i det fall avliden eventet skpaats av misstag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +220,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +245,13 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -183,14 +259,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -217,18 +346,38 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -509,7 +658,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD14"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,19 +670,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" t="s">
         <v>22</v>
       </c>
@@ -610,7 +759,7 @@
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -660,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,11 +830,11 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" t="s">
         <v>22</v>
       </c>
@@ -762,7 +911,7 @@
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -828,4 +977,667 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="34.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E5:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="34.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E5:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>